<commit_message>
key field im meta instead of variable
</commit_message>
<xml_diff>
--- a/src/test/resources/ed/biordm/sbol/toolkit/meta/meta_test.xlsx
+++ b/src/test/resources/ed/biordm/sbol/toolkit/meta/meta_test.xlsx
@@ -33,9 +33,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>variable</t>
-  </si>
-  <si>
     <t>left</t>
   </si>
   <si>
@@ -58,6 +55,9 @@
   </si>
   <si>
     <t>cs0003_slr0613</t>
+  </si>
+  <si>
+    <t>key</t>
   </si>
 </sst>
 </file>
@@ -378,7 +378,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:F7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,7 +394,7 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -403,12 +403,12 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="str">
         <f>CONCATENATE("N ",A2)</f>
@@ -418,15 +418,15 @@
         <v>123</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="str">
         <f>CONCATENATE("N ",A3)</f>
@@ -435,15 +435,15 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="str">
         <f>CONCATENATE("N ",A5)</f>

</xml_diff>